<commit_message>
Added .csv files for scenario development
</commit_message>
<xml_diff>
--- a/MESSAGEix_South_Africa/Data/SSP5/SSP5_excel_draft_demand.xlsx
+++ b/MESSAGEix_South_Africa/Data/SSP5/SSP5_excel_draft_demand.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jansn\GitHub\SSP5_Clone\message_ix_South-Africa_SSP5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Documents/GitHub/SSP5/MESSAGEix_South_Africa/Data/SSP5/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB23234-2182-0E40-8E83-014A583B4B35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25400" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Draft" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -110,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -481,26 +488,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14:N56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
-    <col min="2" max="2" width="22.77734375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" style="6" customWidth="1"/>
-    <col min="4" max="7" width="8.88671875" style="6"/>
-    <col min="8" max="8" width="8.88671875" style="7"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="5"/>
-    <col min="11" max="11" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="8.83203125" style="5"/>
+    <col min="2" max="2" width="22.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="6" customWidth="1"/>
+    <col min="4" max="7" width="8.83203125" style="6"/>
+    <col min="8" max="8" width="8.83203125" style="7"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="5"/>
+    <col min="11" max="11" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="112" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -558,7 +565,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -588,7 +595,7 @@
         <v>0.10319453863187504</v>
       </c>
       <c r="J2" s="5">
-        <f>S2*I2</f>
+        <f t="shared" ref="J2:J8" si="0">S2*I2</f>
         <v>5.3052060000000001</v>
       </c>
       <c r="K2" s="7" t="s">
@@ -605,7 +612,7 @@
         <v>4.0129788722232771</v>
       </c>
       <c r="Q2">
-        <f>$P2/$U$2</f>
+        <f t="shared" ref="Q2:Q11" si="1">$P2/$U$2</f>
         <v>127.25072527344231</v>
       </c>
       <c r="R2">
@@ -624,7 +631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -650,11 +657,11 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I8" si="0">G3/O3</f>
+        <f t="shared" ref="I3:I8" si="2">G3/O3</f>
         <v>7.9723067200406686E-2</v>
       </c>
       <c r="J3" s="5">
-        <f>S3*I3</f>
+        <f t="shared" si="0"/>
         <v>5.6866370000000002</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -664,14 +671,14 @@
         <v>2020</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O8" si="1">G3+G10+G17+G24+G31+G38</f>
+        <f t="shared" ref="O3:O8" si="3">G3+G10+G17+G24+G31+G38</f>
         <v>71.329882300000008</v>
       </c>
       <c r="P3">
         <v>5.879544037458512</v>
       </c>
       <c r="Q3">
-        <f>$P3/$U$2</f>
+        <f t="shared" si="1"/>
         <v>186.43911838719279</v>
       </c>
       <c r="R3">
@@ -679,11 +686,11 @@
         <v>0.38259075089522587</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S11" si="2">Q3*R3</f>
+        <f t="shared" ref="S3:S11" si="4">Q3*R3</f>
         <v>71.329882300000008</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -709,11 +716,11 @@
         <v>10</v>
       </c>
       <c r="I4">
+        <f t="shared" si="2"/>
+        <v>7.3179274968661667E-2</v>
+      </c>
+      <c r="J4" s="5">
         <f t="shared" si="0"/>
-        <v>7.3179274968661667E-2</v>
-      </c>
-      <c r="J4" s="5">
-        <f>S4*I4</f>
         <v>6.9691261834873925</v>
       </c>
       <c r="K4" s="7" t="s">
@@ -723,14 +730,14 @@
         <v>2030</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>92.5621838</v>
       </c>
       <c r="P4">
         <v>6.6401539078103307</v>
       </c>
       <c r="Q4">
-        <f>$P4/$U$2</f>
+        <f t="shared" si="1"/>
         <v>210.5578991568471</v>
       </c>
       <c r="R4">
@@ -738,11 +745,11 @@
         <v>0.45229177158765194</v>
       </c>
       <c r="S4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>95.233605231424534</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -768,11 +775,11 @@
         <v>10</v>
       </c>
       <c r="I5">
+        <f t="shared" si="2"/>
+        <v>6.5905253629870958E-2</v>
+      </c>
+      <c r="J5" s="5">
         <f t="shared" si="0"/>
-        <v>6.5905253629870958E-2</v>
-      </c>
-      <c r="J5" s="5">
-        <f>S5*I5</f>
         <v>8.2354355566160873</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -782,14 +789,14 @@
         <v>2040</v>
       </c>
       <c r="O5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>114.15445030000001</v>
       </c>
       <c r="P5">
         <v>7.5762904751440932</v>
       </c>
       <c r="Q5">
-        <f>$P5/$U$2</f>
+        <f t="shared" si="1"/>
         <v>240.24259497539614</v>
       </c>
       <c r="R5">
@@ -797,11 +804,11 @@
         <v>0.52013553732579965</v>
       </c>
       <c r="S5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>124.95871122607213</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -827,11 +834,11 @@
         <v>10</v>
       </c>
       <c r="I6">
+        <f t="shared" si="2"/>
+        <v>6.032787742996424E-2</v>
+      </c>
+      <c r="J6" s="5">
         <f t="shared" si="0"/>
-        <v>6.032787742996424E-2</v>
-      </c>
-      <c r="J6" s="5">
-        <f>S6*I6</f>
         <v>9.413720115725285</v>
       </c>
       <c r="K6" s="7" t="s">
@@ -841,26 +848,26 @@
         <v>2050</v>
       </c>
       <c r="O6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>135.13042970000001</v>
       </c>
       <c r="P6">
         <v>8.2268859353878856</v>
       </c>
       <c r="Q6">
-        <f>$P6/$U$2</f>
+        <f t="shared" si="1"/>
         <v>260.8728416853084</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6:R11" si="3">R5*(1+$V$2/100)</f>
+        <f t="shared" ref="R6:R11" si="5">R5*(1+$V$2/100)</f>
         <v>0.59815586792466957</v>
       </c>
       <c r="S6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>156.04262103625058</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -886,11 +893,11 @@
         <v>10</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>5.6249363655198115E-2</v>
+      </c>
+      <c r="J7" s="5">
         <f t="shared" si="0"/>
-        <v>5.6249363655198115E-2</v>
-      </c>
-      <c r="J7" s="5">
-        <f>S7*I7</f>
         <v>10.0925950303499</v>
       </c>
       <c r="K7" s="7" t="s">
@@ -900,26 +907,26 @@
         <v>2060</v>
       </c>
       <c r="O7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>156.10640599999999</v>
       </c>
       <c r="P7">
         <v>8.2258281600965404</v>
       </c>
       <c r="Q7">
-        <f>$P7/$U$2</f>
+        <f t="shared" si="1"/>
         <v>260.83929985085427</v>
       </c>
       <c r="R7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.68787924811336998</v>
       </c>
       <c r="S7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>179.42594145982349</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -945,11 +952,11 @@
         <v>10</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
+        <v>5.3137071456265762E-2</v>
+      </c>
+      <c r="J8" s="5">
         <f t="shared" si="0"/>
-        <v>5.3137071456265762E-2</v>
-      </c>
-      <c r="J8" s="5">
-        <f>S8*I8</f>
         <v>10.563926268531496</v>
       </c>
       <c r="K8" s="7" t="s">
@@ -959,26 +966,26 @@
         <v>2070</v>
       </c>
       <c r="O8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>177.0823785</v>
       </c>
       <c r="P8">
         <v>7.925456828005002</v>
       </c>
       <c r="Q8">
-        <f>$P8/$U$2</f>
+        <f t="shared" si="1"/>
         <v>251.31458739234532</v>
       </c>
       <c r="R8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.79106113533037536</v>
       </c>
       <c r="S8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>198.80520282767353</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1008,7 +1015,7 @@
         <v>0.19056581585959886</v>
       </c>
       <c r="J9" s="5">
-        <f>I9*S2</f>
+        <f t="shared" ref="J9:J15" si="6">I9*S2</f>
         <v>9.7969419999999996</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -1021,19 +1028,19 @@
         <v>7.4400845833968017</v>
       </c>
       <c r="Q9">
-        <f>$P9/$U$2</f>
+        <f t="shared" si="1"/>
         <v>235.92353448112638</v>
       </c>
       <c r="R9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.90972030562993156</v>
       </c>
       <c r="S9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>214.624429893464</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1059,11 +1066,11 @@
         <v>10</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I15" si="4">G10/O3</f>
+        <f t="shared" ref="I10:I15" si="7">G10/O3</f>
         <v>0.18823575151195782</v>
       </c>
       <c r="J10" s="5">
-        <f>I10*S3</f>
+        <f t="shared" si="6"/>
         <v>13.426833999999999</v>
       </c>
       <c r="K10" s="7" t="s">
@@ -1076,19 +1083,19 @@
         <v>6.6669617370726604</v>
       </c>
       <c r="Q10">
-        <f>$P10/$U$2</f>
+        <f t="shared" si="1"/>
         <v>211.40796984629185</v>
       </c>
       <c r="R10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0461783514744212</v>
       </c>
       <c r="S10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>221.17044138234775</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1114,11 +1121,11 @@
         <v>10</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.19191107286731929</v>
       </c>
       <c r="J11" s="5">
-        <f>I11*S4</f>
+        <f t="shared" si="6"/>
         <v>18.276383352985434</v>
       </c>
       <c r="K11" s="7" t="s">
@@ -1131,19 +1138,19 @@
         <v>6.0266616135465583</v>
       </c>
       <c r="Q11">
-        <f>$P11/$U$2</f>
+        <f t="shared" si="1"/>
         <v>191.1041861221004</v>
       </c>
       <c r="R11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2031051041955843</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>229.91842175664192</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1169,18 +1176,18 @@
         <v>10</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.18711109329392475</v>
       </c>
       <c r="J12" s="5">
-        <f>I12*S5</f>
+        <f t="shared" si="6"/>
         <v>23.381161074110185</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -1206,18 +1213,18 @@
         <v>10</v>
       </c>
       <c r="I13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.17656071288286593</v>
       </c>
       <c r="J13" s="5">
-        <f>I13*S6</f>
+        <f t="shared" si="6"/>
         <v>27.550996410271292</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -1243,18 +1250,22 @@
         <v>10</v>
       </c>
       <c r="I14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.16884563340725428</v>
       </c>
       <c r="J14" s="5">
-        <f>I14*S7</f>
+        <f t="shared" si="6"/>
         <v>30.295286735476825</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N14" t="str">
+        <f>A1&amp;";"&amp;B1&amp;";"&amp;C1&amp;";"&amp;D1&amp;";"&amp;E1&amp;";"&amp;F1&amp;";"&amp;G1&amp;";"&amp;H1&amp;";"&amp;I1&amp;";"&amp;J1&amp;";"&amp;K1</f>
+        <v>;node;commodity;level;year;time;value;unit;share of total in year;SSP5 value final energy;Unit</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -1280,18 +1291,22 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.1629583149065281</v>
       </c>
       <c r="J15" s="5">
-        <f>I15*S8</f>
+        <f t="shared" si="6"/>
         <v>32.396960847448213</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N15" t="str">
+        <f t="shared" ref="N15:N78" si="8">A2&amp;";"&amp;B2&amp;";"&amp;C2&amp;";"&amp;D2&amp;";"&amp;E2&amp;";"&amp;F2&amp;";"&amp;G2&amp;";"&amp;H2&amp;";"&amp;I2&amp;";"&amp;J2&amp;";"&amp;K2</f>
+        <v>0;South Africa;i_feed;useful;2010;year;5,305206;GWa;0,103194538631875;5,305206;GWa</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -1321,14 +1336,18 @@
         <v>0.16964186884724633</v>
       </c>
       <c r="J16" s="5">
-        <f>I16*S2</f>
+        <f t="shared" ref="J16:J22" si="9">I16*S2</f>
         <v>8.721247</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N16" t="str">
+        <f t="shared" si="8"/>
+        <v>1;South Africa;i_feed;useful;2020;year;5,686637;GWa;0,0797230672004067;5,686637;GWa</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -1354,18 +1373,22 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:I22" si="5">G17/O3</f>
+        <f t="shared" ref="I17:I22" si="10">G17/O3</f>
         <v>0.15900058480819895</v>
       </c>
       <c r="J17" s="5">
-        <f>I17*S3</f>
+        <f t="shared" si="9"/>
         <v>11.341493</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N17" t="str">
+        <f t="shared" si="8"/>
+        <v>2;South Africa;i_feed;useful;2030;year;6,7736335;GWa;0,0731792749686617;6,96912618348739;GWa</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -1391,18 +1414,22 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.14829721422367736</v>
       </c>
       <c r="J18" s="5">
-        <f>I18*S4</f>
+        <f t="shared" si="9"/>
         <v>14.122878356297685</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N18" t="str">
+        <f t="shared" si="8"/>
+        <v>3;South Africa;i_feed;useful;2040;year;7,523378;GWa;0,065905253629871;8,23543555661609;GWa</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -1428,18 +1455,22 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.13743312642450697</v>
       </c>
       <c r="J19" s="5">
-        <f>I19*S5</f>
+        <f t="shared" si="9"/>
         <v>17.173466357776228</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N19" t="str">
+        <f t="shared" si="8"/>
+        <v>4;South Africa;i_feed;useful;2050;year;8,152132;GWa;0,0603278774299642;9,41372011572528;GWa</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -1465,18 +1496,22 @@
         <v>10</v>
       </c>
       <c r="I20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.1248985297942851</v>
       </c>
       <c r="J20" s="5">
-        <f>I20*S6</f>
+        <f t="shared" si="9"/>
         <v>19.489493952674483</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N20" t="str">
+        <f t="shared" si="8"/>
+        <v>5;South Africa;i_feed;useful;2060;year;8,780886;GWa;0,0562493636551981;10,0925950303499;GWa</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -1502,18 +1537,22 @@
         <v>10</v>
       </c>
       <c r="I21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.11573248313717505</v>
       </c>
       <c r="J21" s="5">
-        <f>I21*S7</f>
+        <f t="shared" si="9"/>
         <v>20.765409744370778</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N21" t="str">
+        <f t="shared" si="8"/>
+        <v>6;South Africa;i_feed;useful;2070;year;9,409639;GWa;0,0531370714562658;10,5639262685315;GWa</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -1539,18 +1578,22 @@
         <v>10</v>
       </c>
       <c r="I22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.10873792843255717</v>
       </c>
       <c r="J22" s="5">
-        <f>I22*S8</f>
+        <f t="shared" si="9"/>
         <v>21.617665917095575</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N22" t="str">
+        <f t="shared" si="8"/>
+        <v>7;South Africa;i_spec;useful;2010;year;9,796942;GWa;0,190565815859599;9,796942;GWa</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -1580,14 +1623,18 @@
         <v>7.3944944165315094E-2</v>
       </c>
       <c r="J23" s="5">
-        <f>I23*S2</f>
+        <f t="shared" ref="J23:J29" si="11">I23*S2</f>
         <v>3.8014915</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N23" t="str">
+        <f t="shared" si="8"/>
+        <v>8;South Africa;i_spec;useful;2020;year;13,426834;GWa;0,188235751511958;13,426834;GWa</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -1613,18 +1660,22 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I29" si="6">G24/O3</f>
+        <f t="shared" ref="I24:I29" si="12">G24/O3</f>
         <v>0.10125504300741008</v>
       </c>
       <c r="J24" s="5">
-        <f>I24*S3</f>
+        <f t="shared" si="11"/>
         <v>7.2225102999999997</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N24" t="str">
+        <f t="shared" si="8"/>
+        <v>9;South Africa;i_spec;useful;2030;year;17,763708;GWa;0,191911072867319;18,2763833529854;GWa</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -1650,18 +1701,22 @@
         <v>10</v>
       </c>
       <c r="I25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.13423314457280555</v>
       </c>
       <c r="J25" s="5">
-        <f>I25*S4</f>
+        <f t="shared" si="11"/>
         <v>12.783506299219301</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N25" t="str">
+        <f t="shared" si="8"/>
+        <v>10;South Africa;i_spec;useful;2040;year;21,359564;GWa;0,187111093293925;23,3811610741102;GWa</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -1687,18 +1742,22 @@
         <v>10</v>
       </c>
       <c r="I26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.16681525731108532</v>
       </c>
       <c r="J26" s="5">
-        <f>I26*S5</f>
+        <f t="shared" si="11"/>
         <v>20.845019566438829</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N26" t="str">
+        <f t="shared" si="8"/>
+        <v>11;South Africa;i_spec;useful;2050;year;23,858725;GWa;0,176560712882866;27,5509964102713;GWa</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -1724,18 +1783,22 @@
         <v>10</v>
       </c>
       <c r="I27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.19684581821469629</v>
       </c>
       <c r="J27" s="5">
-        <f>I27*S6</f>
+        <f t="shared" si="11"/>
         <v>30.716337414246524</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N27" t="str">
+        <f t="shared" si="8"/>
+        <v>12;South Africa;i_spec;useful;2060;year;26,357885;GWa;0,168845633407254;30,2952867354768;GWa</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -1761,18 +1824,22 @@
         <v>10</v>
       </c>
       <c r="I28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.21880596623305773</v>
       </c>
       <c r="J28" s="5">
-        <f>I28*S7</f>
+        <f t="shared" si="11"/>
         <v>39.259466488392732</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N28" t="str">
+        <f t="shared" si="8"/>
+        <v>13;South Africa;i_spec;useful;2070;year;28,857046;GWa;0,162958314906528;32,3969608474482;GWa</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -1798,18 +1865,22 @@
         <v>10</v>
       </c>
       <c r="I29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.23556361368841677</v>
       </c>
       <c r="J29" s="5">
-        <f>I29*S8</f>
+        <f t="shared" si="11"/>
         <v>46.831271998145425</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N29" t="str">
+        <f t="shared" si="8"/>
+        <v>14;South Africa;i_therm;useful;2010;year;8,721247;GWa;0,169641868847246;8,721247;GWa</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -1839,14 +1910,18 @@
         <v>8.4052412970530468E-2</v>
       </c>
       <c r="J30" s="5">
-        <f>I30*S2</f>
+        <f t="shared" ref="J30:J36" si="13">I30*S2</f>
         <v>4.3211139999999997</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N30" t="str">
+        <f t="shared" si="8"/>
+        <v>15;South Africa;i_therm;useful;2020;year;11,341493;GWa;0,159000584808199;11,341493;GWa</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -1872,18 +1947,22 @@
         <v>10</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:I36" si="7">G31/O3</f>
+        <f t="shared" ref="I31:I36" si="14">G31/O3</f>
         <v>0.10770578546153019</v>
       </c>
       <c r="J31" s="5">
-        <f>I31*S3</f>
+        <f t="shared" si="13"/>
         <v>7.6826410000000003</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N31" t="str">
+        <f t="shared" si="8"/>
+        <v>16;South Africa;i_therm;useful;2030;year;13,726714;GWa;0,148297214223677;14,1228783562977;GWa</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -1909,18 +1988,22 @@
         <v>10</v>
       </c>
       <c r="I32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>7.9854590682204712E-2</v>
       </c>
       <c r="J32" s="5">
-        <f>I32*S4</f>
+        <f t="shared" si="13"/>
         <v>7.6048405649460751</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N32" t="str">
+        <f t="shared" si="8"/>
+        <v>17;South Africa;i_therm;useful;2040;year;15,688603;GWa;0,137433126424507;17,1734663577762;GWa</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -1946,18 +2029,22 @@
         <v>10</v>
       </c>
       <c r="I33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>5.8433090277865404E-2</v>
       </c>
       <c r="J33" s="5">
-        <f>I33*S5</f>
+        <f t="shared" si="13"/>
         <v>7.3017236540787858</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N33" t="str">
+        <f t="shared" si="8"/>
+        <v>18;South Africa;i_therm;useful;2050;year;16,877592;GWa;0,124898529794285;19,4894939526745;GWa</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -1983,18 +2070,22 @@
         <v>10</v>
       </c>
       <c r="I34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>4.6328060333252971E-2</v>
       </c>
       <c r="J34" s="5">
-        <f>I34*S6</f>
+        <f t="shared" si="13"/>
         <v>7.2291519619263465</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N34" t="str">
+        <f t="shared" si="8"/>
+        <v>19;South Africa;i_therm;useful;2060;year;18,066582;GWa;0,115732483137175;20,7654097443708;GWa</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -2020,18 +2111,22 @@
         <v>10</v>
       </c>
       <c r="I35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>3.7476130223637334E-2</v>
       </c>
       <c r="J35" s="5">
-        <f>I35*S7</f>
+        <f t="shared" si="13"/>
         <v>6.7241899476470746</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N35" t="str">
+        <f t="shared" si="8"/>
+        <v>20;South Africa;i_therm;useful;2070;year;19,255571;GWa;0,108737928432557;21,6176659170956;GWa</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -2057,18 +2152,22 @@
         <v>10</v>
       </c>
       <c r="I36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>3.0721280943264491E-2</v>
       </c>
       <c r="J36" s="5">
-        <f>I36*S8</f>
+        <f t="shared" si="13"/>
         <v>6.107550489051639</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N36" t="str">
+        <f t="shared" si="8"/>
+        <v>21;South Africa;rc_spec;useful;2010;year;3,8014915;GWa;0,0739449441653151;3,8014915;GWa</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -2098,14 +2197,18 @@
         <v>0.37860041952543427</v>
       </c>
       <c r="J37" s="5">
-        <f>I37*S2</f>
+        <f t="shared" ref="J37:J43" si="15">I37*S2</f>
         <v>19.463754999999999</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N37" t="str">
+        <f t="shared" si="8"/>
+        <v>22;South Africa;rc_spec;useful;2020;year;7,2225103;GWa;0,10125504300741;7,2225103;GWa</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -2131,18 +2234,22 @@
         <v>10</v>
       </c>
       <c r="I38">
-        <f t="shared" ref="I38:I43" si="8">G38/O3</f>
+        <f t="shared" ref="I38:I43" si="16">G38/O3</f>
         <v>0.36407976801049619</v>
       </c>
       <c r="J38" s="5">
-        <f>I38*S3</f>
+        <f t="shared" si="15"/>
         <v>25.969767000000001</v>
       </c>
       <c r="K38" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N38" t="str">
+        <f t="shared" si="8"/>
+        <v>23;South Africa;rc_spec;useful;2030;year;12,424913;GWa;0,134233144572806;12,7835062992193;GWa</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -2168,18 +2275,22 @@
         <v>10</v>
       </c>
       <c r="I39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.37252470268533139</v>
       </c>
       <c r="J39" s="5">
-        <f>I39*S4</f>
+        <f t="shared" si="15"/>
         <v>35.476870474488642</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N39" t="str">
+        <f t="shared" si="8"/>
+        <v>24;South Africa;rc_spec;useful;2040;year;19,042704;GWa;0,166815257311085;20,8450195664388;GWa</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -2205,18 +2316,22 @@
         <v>10</v>
       </c>
       <c r="I40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.38430217906274655</v>
       </c>
       <c r="J40" s="5">
-        <f>I40*S5</f>
+        <f t="shared" si="15"/>
         <v>48.021905017052006</v>
       </c>
       <c r="K40" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N40" t="str">
+        <f t="shared" si="8"/>
+        <v>25;South Africa;rc_spec;useful;2050;year;26,59986;GWa;0,196845818214696;30,7163374142465;GWa</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -2242,18 +2357,22 @@
         <v>10</v>
       </c>
       <c r="I41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.39503900134493541</v>
       </c>
       <c r="J41" s="5">
-        <f>I41*S6</f>
+        <f t="shared" si="15"/>
         <v>61.642921181406642</v>
       </c>
       <c r="K41" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N41" t="str">
+        <f t="shared" si="8"/>
+        <v>26;South Africa;rc_spec;useful;2060;year;34,157013;GWa;0,218805966233058;39,2594664883927;GWa</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -2279,18 +2398,22 @@
         <v>10</v>
       </c>
       <c r="I42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.40289042334367753</v>
       </c>
       <c r="J42" s="5">
-        <f>I42*S7</f>
+        <f t="shared" si="15"/>
         <v>72.288993513586192</v>
       </c>
       <c r="K42" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N42" t="str">
+        <f t="shared" si="8"/>
+        <v>27;South Africa;rc_spec;useful;2070;year;41,714165;GWa;0,235563613688417;46,8312719981454;GWa</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -2316,15 +2439,97 @@
         <v>10</v>
       </c>
       <c r="I43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0.4088817905729677</v>
       </c>
       <c r="J43" s="5">
-        <f>I43*S8</f>
+        <f t="shared" si="15"/>
         <v>81.287827307401173</v>
       </c>
       <c r="K43" s="7" t="s">
         <v>10</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="8"/>
+        <v>28;South Africa;rc_therm;useful;2010;year;4,321114;GWa;0,0840524129705305;4,321114;GWa</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N44" t="str">
+        <f t="shared" si="8"/>
+        <v>29;South Africa;rc_therm;useful;2020;year;7,682641;GWa;0,10770578546153;7,682641;GWa</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N45" t="str">
+        <f t="shared" si="8"/>
+        <v>30;South Africa;rc_therm;useful;2030;year;7,3915153;GWa;0,0798545906822047;7,60484056494608;GWa</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N46" t="str">
+        <f t="shared" si="8"/>
+        <v>31;South Africa;rc_therm;useful;2040;year;6,6703973;GWa;0,0584330902778654;7,30172365407879;GWa</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N47" t="str">
+        <f t="shared" si="8"/>
+        <v>32;South Africa;rc_therm;useful;2050;year;6,2603307;GWa;0,046328060333253;7,22915196192635;GWa</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N48" t="str">
+        <f t="shared" si="8"/>
+        <v>33;South Africa;rc_therm;useful;2060;year;5,850264;GWa;0,0374761302236373;6,72418994764707;GWa</v>
+      </c>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N49" t="str">
+        <f t="shared" si="8"/>
+        <v>34;South Africa;rc_therm;useful;2070;year;5,4401975;GWa;0,0307212809432645;6,10755048905164;GWa</v>
+      </c>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N50" t="str">
+        <f t="shared" si="8"/>
+        <v>35;South Africa;transport;useful;2010;year;19,463755;GWa;0,378600419525434;19,463755;GWa</v>
+      </c>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N51" t="str">
+        <f t="shared" si="8"/>
+        <v>36;South Africa;transport;useful;2020;year;25,969767;GWa;0,364079768010496;25,969767;GWa</v>
+      </c>
+    </row>
+    <row r="52" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N52" t="str">
+        <f t="shared" si="8"/>
+        <v>37;South Africa;transport;useful;2030;year;34,4817;GWa;0,372524702685331;35,4768704744886;GWa</v>
+      </c>
+    </row>
+    <row r="53" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N53" t="str">
+        <f t="shared" si="8"/>
+        <v>38;South Africa;transport;useful;2040;year;43,869804;GWa;0,384302179062747;48,021905017052;GWa</v>
+      </c>
+    </row>
+    <row r="54" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N54" t="str">
+        <f t="shared" si="8"/>
+        <v>39;South Africa;transport;useful;2050;year;53,38179;GWa;0,395039001344935;61,6429211814066;GWa</v>
+      </c>
+    </row>
+    <row r="55" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N55" t="str">
+        <f t="shared" si="8"/>
+        <v>40;South Africa;transport;useful;2060;year;62,893776;GWa;0,402890423343678;72,2889935135862;GWa</v>
+      </c>
+    </row>
+    <row r="56" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N56" t="str">
+        <f t="shared" si="8"/>
+        <v>41;South Africa;transport;useful;2070;year;72,40576;GWa;0,408881790572968;81,2878273074012;GWa</v>
       </c>
     </row>
   </sheetData>

</xml_diff>